<commit_message>
updates to code to change to louisiana
</commit_message>
<xml_diff>
--- a/state_list.xlsx
+++ b/state_list.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>OK</t>
+    <t>LA</t>
   </si>
   <si>
-    <t>40</t>
+    <t>22</t>
   </si>
 </sst>
 </file>

</xml_diff>